<commit_message>
primeira versão do brownian bridge
</commit_message>
<xml_diff>
--- a/R/book1.xlsx
+++ b/R/book1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>increm</t>
   </si>
@@ -34,11 +34,33 @@
   <si>
     <t>brown</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>vals</t>
+  </si>
+  <si>
+    <t>t´s</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,9 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,91 +188,91 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2926387174799454E-2</c:v>
+                  <c:v>-0.26359371625231715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.4803645499071278E-2</c:v>
+                  <c:v>0.26782533050381319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.3329404377525179E-2</c:v>
+                  <c:v>-0.33403322806540903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23512347159000999</c:v>
+                  <c:v>-0.51516526477143354</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2312674112440973E-3</c:v>
+                  <c:v>-9.6058696029611753E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.16277202903684726</c:v>
+                  <c:v>-0.16767770795167561</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.16274010060165081</c:v>
+                  <c:v>0.13579114887987659</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.21545570658086022</c:v>
+                  <c:v>-0.23709035612942692</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21429932689384393</c:v>
+                  <c:v>3.1437299644823551E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-9.8050988306628895E-2</c:v>
+                  <c:v>-0.1092859135743057</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.22472596310084317</c:v>
+                  <c:v>-0.20903012136703045</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.12916390470723604</c:v>
+                  <c:v>-4.9254575786512531E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.13100032761621222</c:v>
+                  <c:v>0.14234795029263586</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1593604990892016E-2</c:v>
+                  <c:v>0.18030345190026853</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3582831673815509E-2</c:v>
+                  <c:v>-0.16499953018411631</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.11098732919586378</c:v>
+                  <c:v>0.1061477213555355</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.17446424062260493</c:v>
+                  <c:v>-0.23518421565672235</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.20623497686179901</c:v>
+                  <c:v>4.5400871114152884E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.34763457354801242</c:v>
+                  <c:v>0.13477596248169701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.8293865779871369E-2</c:v>
+                  <c:v>0.18150198730863021</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.23437419102882728</c:v>
+                  <c:v>9.6181474628406829E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.28911990446244673</c:v>
+                  <c:v>2.9598858603923469E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.8134121167253285E-2</c:v>
+                  <c:v>-0.17563298037015523</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.13964305385693682</c:v>
+                  <c:v>0.14311151773348635</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.13247681813538717</c:v>
+                  <c:v>0.21916955176459083</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.13146916232180736</c:v>
+                  <c:v>-0.28149711149902035</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.10123895160972526</c:v>
+                  <c:v>2.6092018245250842E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.18156986095997171</c:v>
+                  <c:v>-7.7574149761208064E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.30656903101739308</c:v>
+                  <c:v>9.2447259962898626E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -494,91 +518,91 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2926387174799454E-2</c:v>
+                  <c:v>-0.26359371625231715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1877258324271825E-2</c:v>
+                  <c:v>4.2316142514960409E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.5206662701797002E-2</c:v>
+                  <c:v>-0.32980161381391299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19991680888821298</c:v>
+                  <c:v>-0.84496687858534658</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20514807629945708</c:v>
+                  <c:v>-0.85457274818830775</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.2376047262609823E-2</c:v>
+                  <c:v>-1.0222504561399834</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.12036405333904099</c:v>
+                  <c:v>-0.8864593072601068</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.33581975991990121</c:v>
+                  <c:v>-1.1235496633895337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.12152043302605728</c:v>
+                  <c:v>-1.0921123637447101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.21957142133268617</c:v>
+                  <c:v>-1.2013982773190157</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.44429738443352934</c:v>
+                  <c:v>-1.4104283986860462</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.3151334797262933</c:v>
+                  <c:v>-1.4596829744725588</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.18413315211008108</c:v>
+                  <c:v>-1.3173350241799229</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.17253954711918906</c:v>
+                  <c:v>-1.1370315722796542</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.14895671544537356</c:v>
+                  <c:v>-1.3020311024637705</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-3.7969386249509782E-2</c:v>
+                  <c:v>-1.195883381108235</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.2124336268721147</c:v>
+                  <c:v>-1.4310675967649573</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-6.1986500103156927E-3</c:v>
+                  <c:v>-1.3856667256508044</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.35383322355832814</c:v>
+                  <c:v>-1.2508907631691073</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.41212708933819953</c:v>
+                  <c:v>-1.0693887758604772</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.64650128036702681</c:v>
+                  <c:v>-0.97320730123207033</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.93562118482947354</c:v>
+                  <c:v>-0.94360844262814692</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.87748706366222029</c:v>
+                  <c:v>-1.1192414229983021</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-1.0171301175191572</c:v>
+                  <c:v>-0.9761299052648158</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.88465329938377002</c:v>
+                  <c:v>-0.75696035350022495</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.75318413706196263</c:v>
+                  <c:v>-1.0384574649992453</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.85442308867168792</c:v>
+                  <c:v>-1.0123654467539944</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.67285322771171618</c:v>
+                  <c:v>-1.0899395965152026</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.36628419669432311</c:v>
+                  <c:v>-0.99749233655230396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2188,15 +2212,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2207,7 +2236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2218,187 +2247,190 @@
         <f>SUM($B$2:B2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <f ca="1">_xlfn.NORM.INV(RAND(),0,SQRT(1/30))</f>
-        <v>1.2926387174799454E-2</v>
+        <v>-0.26359371625231715</v>
       </c>
       <c r="C3" s="1">
         <f ca="1">SUM($B$2:B3)</f>
-        <v>1.2926387174799454E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-0.26359371625231715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B31" ca="1" si="0">_xlfn.NORM.INV(RAND(),0,SQRT(1/30))</f>
-        <v>-3.4803645499071278E-2</v>
+        <v>0.26782533050381319</v>
       </c>
       <c r="C4" s="1">
         <f ca="1">SUM($B$2:B4)</f>
-        <v>-2.1877258324271825E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.2316142514960409E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3329404377525179E-2</v>
+        <v>-0.33403322806540903</v>
       </c>
       <c r="C5" s="1">
         <f ca="1">SUM($B$2:B5)</f>
-        <v>-3.5206662701797002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-0.32980161381391299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23512347159000999</v>
+        <v>-0.51516526477143354</v>
       </c>
       <c r="C6" s="1">
         <f ca="1">SUM($B$2:B6)</f>
-        <v>0.19991680888821298</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-0.84496687858534658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2312674112440973E-3</v>
+        <v>-9.6058696029611753E-3</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">SUM($B$2:B7)</f>
-        <v>0.20514807629945708</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-0.85457274818830775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16277202903684726</v>
+        <v>-0.16767770795167561</v>
       </c>
       <c r="C8" s="1">
         <f ca="1">SUM($B$2:B8)</f>
-        <v>4.2376047262609823E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.0222504561399834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16274010060165081</v>
+        <v>0.13579114887987659</v>
       </c>
       <c r="C9" s="1">
         <f ca="1">SUM($B$2:B9)</f>
-        <v>-0.12036405333904099</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-0.8864593072601068</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.21545570658086022</v>
+        <v>-0.23709035612942692</v>
       </c>
       <c r="C10" s="1">
         <f ca="1">SUM($B$2:B10)</f>
-        <v>-0.33581975991990121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.1235496633895337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21429932689384393</v>
+        <v>3.1437299644823551E-2</v>
       </c>
       <c r="C11" s="1">
         <f ca="1">SUM($B$2:B11)</f>
-        <v>-0.12152043302605728</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.0921123637447101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.8050988306628895E-2</v>
+        <v>-0.1092859135743057</v>
       </c>
       <c r="C12" s="1">
         <f ca="1">SUM($B$2:B12)</f>
-        <v>-0.21957142133268617</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.2013982773190157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22472596310084317</v>
+        <v>-0.20903012136703045</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">SUM($B$2:B13)</f>
-        <v>-0.44429738443352934</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.4104283986860462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12916390470723604</v>
+        <v>-4.9254575786512531E-2</v>
       </c>
       <c r="C14" s="1">
         <f ca="1">SUM($B$2:B14)</f>
-        <v>-0.3151334797262933</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.4596829744725588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13100032761621222</v>
+        <v>0.14234795029263586</v>
       </c>
       <c r="C15" s="1">
         <f ca="1">SUM($B$2:B15)</f>
-        <v>-0.18413315211008108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1.3173350241799229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1593604990892016E-2</v>
+        <v>0.18030345190026853</v>
       </c>
       <c r="C16" s="1">
         <f ca="1">SUM($B$2:B16)</f>
-        <v>-0.17253954711918906</v>
+        <v>-1.1370315722796542</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2407,11 +2439,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3582831673815509E-2</v>
+        <v>-0.16499953018411631</v>
       </c>
       <c r="C17" s="1">
         <f ca="1">SUM($B$2:B17)</f>
-        <v>-0.14895671544537356</v>
+        <v>-1.3020311024637705</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2420,11 +2452,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11098732919586378</v>
+        <v>0.1061477213555355</v>
       </c>
       <c r="C18" s="1">
         <f ca="1">SUM($B$2:B18)</f>
-        <v>-3.7969386249509782E-2</v>
+        <v>-1.195883381108235</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2433,11 +2465,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17446424062260493</v>
+        <v>-0.23518421565672235</v>
       </c>
       <c r="C19" s="1">
         <f ca="1">SUM($B$2:B19)</f>
-        <v>-0.2124336268721147</v>
+        <v>-1.4310675967649573</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,11 +2478,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20623497686179901</v>
+        <v>4.5400871114152884E-2</v>
       </c>
       <c r="C20" s="1">
         <f ca="1">SUM($B$2:B20)</f>
-        <v>-6.1986500103156927E-3</v>
+        <v>-1.3856667256508044</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,11 +2491,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.34763457354801242</v>
+        <v>0.13477596248169701</v>
       </c>
       <c r="C21" s="1">
         <f ca="1">SUM($B$2:B21)</f>
-        <v>-0.35383322355832814</v>
+        <v>-1.2508907631691073</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2472,11 +2504,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8293865779871369E-2</v>
+        <v>0.18150198730863021</v>
       </c>
       <c r="C22" s="1">
         <f ca="1">SUM($B$2:B22)</f>
-        <v>-0.41212708933819953</v>
+        <v>-1.0693887758604772</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,11 +2517,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.23437419102882728</v>
+        <v>9.6181474628406829E-2</v>
       </c>
       <c r="C23" s="1">
         <f ca="1">SUM($B$2:B23)</f>
-        <v>-0.64650128036702681</v>
+        <v>-0.97320730123207033</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2498,11 +2530,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28911990446244673</v>
+        <v>2.9598858603923469E-2</v>
       </c>
       <c r="C24" s="1">
         <f ca="1">SUM($B$2:B24)</f>
-        <v>-0.93562118482947354</v>
+        <v>-0.94360844262814692</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,11 +2543,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8134121167253285E-2</v>
+        <v>-0.17563298037015523</v>
       </c>
       <c r="C25" s="1">
         <f ca="1">SUM($B$2:B25)</f>
-        <v>-0.87748706366222029</v>
+        <v>-1.1192414229983021</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,11 +2556,11 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.13964305385693682</v>
+        <v>0.14311151773348635</v>
       </c>
       <c r="C26" s="1">
         <f ca="1">SUM($B$2:B26)</f>
-        <v>-1.0171301175191572</v>
+        <v>-0.9761299052648158</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,11 +2569,11 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13247681813538717</v>
+        <v>0.21916955176459083</v>
       </c>
       <c r="C27" s="1">
         <f ca="1">SUM($B$2:B27)</f>
-        <v>-0.88465329938377002</v>
+        <v>-0.75696035350022495</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,11 +2582,11 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13146916232180736</v>
+        <v>-0.28149711149902035</v>
       </c>
       <c r="C28" s="1">
         <f ca="1">SUM($B$2:B28)</f>
-        <v>-0.75318413706196263</v>
+        <v>-1.0384574649992453</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2563,11 +2595,11 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10123895160972526</v>
+        <v>2.6092018245250842E-2</v>
       </c>
       <c r="C29" s="1">
         <f ca="1">SUM($B$2:B29)</f>
-        <v>-0.85442308867168792</v>
+        <v>-1.0123654467539944</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2576,11 +2608,11 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18156986095997171</v>
+        <v>-7.7574149761208064E-2</v>
       </c>
       <c r="C30" s="1">
         <f ca="1">SUM($B$2:B30)</f>
-        <v>-0.67285322771171618</v>
+        <v>-1.0899395965152026</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,15 +2621,178 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30656903101739308</v>
+        <v>9.2447259962898626E-2</v>
       </c>
       <c r="C31" s="1">
         <f ca="1">SUM($B$2:B31)</f>
-        <v>-0.36628419669432311</v>
+        <v>-0.99749233655230396</v>
       </c>
       <c r="D31">
         <f ca="1">_xlfn.NORM.INV(RAND(),0,SQRT(1))</f>
-        <v>-0.21436207449190006</v>
+        <v>-0.36870574758846042</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <v>-0.98819970000000001</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <f>_xlfn.FLOOR.MATH((E40+E39)/2, 1)</f>
+        <v>5</v>
+      </c>
+      <c r="F41" s="2">
+        <f>((E40-E41)*F39+(E41-E39)*F40)/(E40-E39)</f>
+        <v>-0.43919986666666666</v>
+      </c>
+      <c r="G41">
+        <f>(((E41-E39)*(E40-E41))/(E40-E39))</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="I41">
+        <f ca="1">F41+G41*_xlfn.NORM.INV(RAND(),0,1)</f>
+        <v>2.5011573874809674</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <f>((E40/10-E41/10)*F39+(E41/10-E39/10)*F40)/(E40/10-E39/10)</f>
+        <v>-0.43919986666666666</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="L45" t="s">
+        <v>3</v>
+      </c>
+      <c r="M45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <f>E41</f>
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>-0.4785201</v>
+      </c>
+      <c r="L46" s="3">
+        <f>J49</f>
+        <v>-0.10979996666666667</v>
+      </c>
+      <c r="M46">
+        <f>-L46</f>
+        <v>0.10979996666666667</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <f>_xlfn.FLOOR.MATH((E46+E45)/2, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="F47" s="2">
+        <f>((E46-E47)*F45+(E47-E45)*F46)/(E46-E45)</f>
+        <v>-0.23926005</v>
+      </c>
+      <c r="G47">
+        <f>SQRT(((E47-E45)*(E46-E47))/(E46-E45))</f>
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47" s="3">
+        <f>K47*$L$46+$M$46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>0.748</v>
+      </c>
+      <c r="K48">
+        <v>5</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" ref="L48:L49" si="1">K48*$L$46+$M$46</f>
+        <v>-0.43919986666666666</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <f>F40/9</f>
+        <v>-0.10979996666666667</v>
+      </c>
+      <c r="K49">
+        <v>10</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.98819970000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <f>J49*5</f>
+        <v>-0.54899983333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>